<commit_message>
Update 리볼트데이 스크립트 (ver.0.12).xlsx
</commit_message>
<xml_diff>
--- a/리볼트데이 스크립트 (ver.0.12).xlsx
+++ b/리볼트데이 스크립트 (ver.0.12).xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4351" uniqueCount="3049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4355" uniqueCount="3053">
   <si>
     <t>EventID</t>
   </si>
@@ -13725,6 +13725,22 @@
   </si>
   <si>
     <t>중간에 튜토리얼이 삽입되는 부분이 있음(월드맵, 격투, 추리 등등)</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>whiteFlash_1s</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>RedFlash_1s</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>화면에 빨간 플래시가 터지는 것을 의미합니다.</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>화면에 하얀 플래시가 터지는 것을 의미합니다.</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -15927,10 +15943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Q17"/>
+  <dimension ref="B3:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -15947,10 +15963,11 @@
     <col min="14" max="14" width="52" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="59.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="61.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37" customWidth="1"/>
+    <col min="17" max="18" width="44" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B3" s="52" t="s">
         <v>3009</v>
       </c>
@@ -15997,10 +16014,16 @@
         <v>3023</v>
       </c>
       <c r="Q3" s="53" t="s">
+        <v>3050</v>
+      </c>
+      <c r="R3" s="53" t="s">
+        <v>3049</v>
+      </c>
+      <c r="S3" s="53" t="s">
         <v>3040</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>3025</v>
       </c>
@@ -16047,35 +16070,41 @@
         <v>3039</v>
       </c>
       <c r="Q4" s="11" t="s">
+        <v>3051</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>3052</v>
+      </c>
+      <c r="S4" s="11" t="s">
         <v>3041</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>3042</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>3043</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>3044</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>3045</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>3046</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
         <v>3048</v>
       </c>

</xml_diff>